<commit_message>
update 31 mei 2024
</commit_message>
<xml_diff>
--- a/assets/format_lampiran.xlsx
+++ b/assets/format_lampiran.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JTIK\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pelayanan_ftik\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70144A09-09B3-49F9-B6A1-ED736045E741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BFFD29-66D5-4901-B022-A4594308D0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{55B3A301-E492-45B7-89C6-223629EFF427}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{55B3A301-E492-45B7-89C6-223629EFF427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>nama</t>
   </si>
@@ -40,6 +41,27 @@
   </si>
   <si>
     <t>lampiran data surat tugas / keterangan</t>
+  </si>
+  <si>
+    <t>Lampiran Pengajuan SK</t>
+  </si>
+  <si>
+    <t>Jabatan</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>Uraian Tugas</t>
+  </si>
+  <si>
+    <t>Lampiran Honorarium (Jika dihonorkan)</t>
+  </si>
+  <si>
+    <t>Kode Akun</t>
+  </si>
+  <si>
+    <t>Nominal</t>
   </si>
 </sst>
 </file>
@@ -393,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8543781-C626-46ED-9E57-EB408DF528B5}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,4 +448,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4491BAE0-6F76-4EFB-A120-F18F22AB1440}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>